<commit_message>
Migration to Automation-Org/TestCases-maintenance/WIP-RMA TestCases
</commit_message>
<xml_diff>
--- a/templates/QARSF/Create Engineering Item Master.xlsx
+++ b/templates/QARSF/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
   <si>
     <t>Item Number</t>
   </si>
@@ -409,6 +409,54 @@
   </si>
   <si>
     <t>a2S1K000002TBSVUA4</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-UEHCR</t>
+  </si>
+  <si>
+    <t>a2S1K000002TBqrUAG</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-UVCY4</t>
+  </si>
+  <si>
+    <t>a2S1K000002TBqwUAG</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-XUL51</t>
+  </si>
+  <si>
+    <t>a2S1K000002TBrBUAW</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-YH5OX</t>
+  </si>
+  <si>
+    <t>a2S1K000002TBrGUAW</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-FNMGQ</t>
+  </si>
+  <si>
+    <t>a2S1K000002TIDSUA4</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-JW530</t>
+  </si>
+  <si>
+    <t>a2S1K000002TIreUAG</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-KMYK0</t>
+  </si>
+  <si>
+    <t>a2S1K000002TIrjUAG</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-QQSVF</t>
+  </si>
+  <si>
+    <t>a2S1K000002TIroUAG</t>
   </si>
 </sst>
 </file>
@@ -419,7 +467,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +495,102 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -481,7 +625,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -495,11 +639,35 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -507,8 +675,24 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="7" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="9" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="13" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="15" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="16" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="17" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="21" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="10" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -943,9 +1127,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.8046875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.03125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.67578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.4921875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.7890625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -967,13 +1151,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RMA End to End Test Cases Other maintenance
</commit_message>
<xml_diff>
--- a/templates/QARSF/Create Engineering Item Master.xlsx
+++ b/templates/QARSF/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="151">
   <si>
     <t>Item Number</t>
   </si>
@@ -457,6 +457,42 @@
   </si>
   <si>
     <t>a2S1K000002TIroUAG</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-VRYT7</t>
+  </si>
+  <si>
+    <t>a2S1K000002TJiJUAW</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-VYWX9</t>
+  </si>
+  <si>
+    <t>a2S1K000002TJiOUAW</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-U9RDG</t>
+  </si>
+  <si>
+    <t>a2S1K000002TLV9UAO</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-VDCA8</t>
+  </si>
+  <si>
+    <t>a2S1K000002TLVEUA4</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-W05D0</t>
+  </si>
+  <si>
+    <t>a2S1K000002TLVJUA4</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-WLQMI</t>
+  </si>
+  <si>
+    <t>a2S1K000002TLVOUA4</t>
   </si>
 </sst>
 </file>
@@ -467,7 +503,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +531,78 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -625,7 +733,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -663,11 +771,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -691,8 +817,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="21" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="10" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="22" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="23" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="24" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="25" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="26" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="27" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="28" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="29" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="30" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="31" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="32" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="33" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1127,9 +1265,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.03125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.59765625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.67578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.7890625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1151,13 +1289,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>